<commit_message>
Add nice!nanos to beta BOM
</commit_message>
<xml_diff>
--- a/BOM/beta/ergoTHWACK beta BOM.xlsx
+++ b/BOM/beta/ergoTHWACK beta BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\ergothwack\BOM\beta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B29195-B499-4595-80C5-E44B1552DB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F4F628-856C-4523-8480-59E9375FB0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{1E54C694-8349-4148-A3EA-D049736EB163}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="106">
   <si>
     <t>vendor</t>
   </si>
@@ -348,6 +348,12 @@
   </si>
   <si>
     <t>battery plate 5052 H32 Aluminum (.063") with deburring</t>
+  </si>
+  <si>
+    <t>typeractive.xyz</t>
+  </si>
+  <si>
+    <t>nice!nano v2.0</t>
   </si>
 </sst>
 </file>
@@ -778,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648A4E3F-A5EF-4889-A125-F0F619BD5235}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -845,8 +851,8 @@
         <v>23.72</v>
       </c>
       <c r="H2" s="5">
-        <f>SUM(G2:G44)</f>
-        <v>561.49000000000012</v>
+        <f>SUM(G2:G100)</f>
+        <v>611.49000000000012</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -866,7 +872,7 @@
         <v>2</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G44" si="0">E3*F3</f>
+        <f t="shared" ref="G3:G45" si="0">E3*F3</f>
         <v>2.68</v>
       </c>
     </row>
@@ -1822,6 +1828,27 @@
       <c r="G44">
         <f t="shared" si="0"/>
         <v>35.86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" t="s">
+        <v>105</v>
+      </c>
+      <c r="D45" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45">
+        <v>25</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>